<commit_message>
Add product code to area inventory report excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/areaInventoryReport.xlsx
+++ b/src/main/resources/excel/areaInventoryReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\jchs-pos\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20EADE3-DFE4-4759-8996-2840E00BA348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A73B8-5138-46FA-9886-0EC941048DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C91B9F7-2FB7-45CF-8412-61317C9D604D}"/>
   </bookViews>
@@ -64,7 +64,7 @@
     <t>Review</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -109,16 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,26 +435,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D7311B-EA7D-4CC2-B62A-D4A2A08A4407}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="3" max="3" width="6.44140625" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -487,33 +483,24 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>